<commit_message>
Add test_data.xlsx for Jenkins tests
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,117 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>harh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>nayak</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>harh1@example.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>9876543212</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>harh123</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>harh123</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>jane</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>smith</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>jane@example.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9876543211</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jane123</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>jane123</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>dave</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>franc</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dave@example.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>9876543215</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>dave123</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>dave123</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -545,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,6 +693,57 @@
         </is>
       </c>
       <c r="C2" t="inlineStr">
+        <is>
+          <t>Login Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>harh1@example.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>harh123</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Login Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>anand1@example.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>anand123</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Login Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>pratham1@example.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>pratham123</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>Login Successful</t>
         </is>
@@ -598,7 +760,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -627,6 +789,41 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>samsung</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sony</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>canon</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>samsung</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>tab</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>